<commit_message>
Added Excel File without filters
</commit_message>
<xml_diff>
--- a/DB_CursoExcel.xlsx
+++ b/DB_CursoExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\000088007\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\000088007\GitFerneyAmaya\DataLiteracy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1461,7 +1461,7 @@
   <dimension ref="A1:J790"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27547,7 +27547,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J790"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel modified the age range
</commit_message>
<xml_diff>
--- a/DB_CursoExcel.xlsx
+++ b/DB_CursoExcel.xlsx
@@ -1461,7 +1461,7 @@
   <dimension ref="A1:J790"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3561,7 +3561,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -8049,7 +8049,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C200" t="s">
         <v>1</v>
@@ -25869,7 +25869,7 @@
         <v>739</v>
       </c>
       <c r="B740" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C740" t="s">
         <v>1</v>

</xml_diff>